<commit_message>
All batche's GPT annoation complete + interannotator agreement for batches 1 and 2 complete
</commit_message>
<xml_diff>
--- a/src/analysis/modified_corpus_batches/xlsx/batch_1.xlsx
+++ b/src/analysis/modified_corpus_batches/xlsx/batch_1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daomingliu/Desktop/mds-cl/523/COLX_523_Group-Repository_David-Daoming-Jacob-Nicole/src/analysis/modified_corpus_batches/xlsx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tkang/Documents/MDS/block5/labs/COLX_523_Group-Repository_David-Daoming-Jacob-Nicole/src/analysis/modified_corpus_batches/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C08FEEE7-C738-0D45-86FF-3DC724790966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{614089B4-58D6-EC49-9F00-91DD85D3E67D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="34560" windowHeight="16460" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="16460" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="961" uniqueCount="655">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="961" uniqueCount="656">
   <si>
     <t>Reviewer</t>
   </si>
@@ -1987,13 +1987,16 @@
   </si>
   <si>
     <t>Logos</t>
+  </si>
+  <si>
+    <t>viewer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2008,12 +2011,30 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FFCCCCCC"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FFCCCCCC"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2062,7 +2083,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -2070,6 +2091,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -5149,10 +5173,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63E80D56-2025-2B49-9EE3-59AD1C97193B}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5161,7 +5185,7 @@
     <col min="4" max="4" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5175,7 +5199,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -5188,8 +5212,9 @@
       <c r="D2" t="s">
         <v>652</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -5202,8 +5227,9 @@
       <c r="D3" t="s">
         <v>653</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -5216,8 +5242,9 @@
       <c r="D4" t="s">
         <v>652</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -5230,8 +5257,9 @@
       <c r="D5" t="s">
         <v>652</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -5244,8 +5272,9 @@
       <c r="D6" t="s">
         <v>652</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -5258,8 +5287,9 @@
       <c r="D7" t="s">
         <v>652</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -5272,8 +5302,9 @@
       <c r="D8" t="s">
         <v>652</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -5286,8 +5317,9 @@
       <c r="D9" t="s">
         <v>654</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -5300,8 +5332,9 @@
       <c r="D10" t="s">
         <v>652</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -5314,8 +5347,9 @@
       <c r="D11" t="s">
         <v>652</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -5328,8 +5362,9 @@
       <c r="D12" t="s">
         <v>652</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -5342,8 +5377,9 @@
       <c r="D13" t="s">
         <v>654</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -5356,8 +5392,9 @@
       <c r="D14" t="s">
         <v>652</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -5370,8 +5407,9 @@
       <c r="D15" t="s">
         <v>652</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>45</v>
       </c>
@@ -5384,8 +5422,9 @@
       <c r="D16" t="s">
         <v>652</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>48</v>
       </c>
@@ -5398,8 +5437,9 @@
       <c r="D17" t="s">
         <v>652</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -5412,8 +5452,9 @@
       <c r="D18" t="s">
         <v>652</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>54</v>
       </c>
@@ -5426,8 +5467,9 @@
       <c r="D19" t="s">
         <v>654</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E19" s="4"/>
+    </row>
+    <row r="20" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>57</v>
       </c>
@@ -5440,8 +5482,9 @@
       <c r="D20" t="s">
         <v>652</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E20" s="4"/>
+    </row>
+    <row r="21" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>60</v>
       </c>
@@ -5454,8 +5497,9 @@
       <c r="D21" t="s">
         <v>652</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E21" s="4"/>
+    </row>
+    <row r="22" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -5466,10 +5510,11 @@
         <v>63</v>
       </c>
       <c r="D22" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+        <v>653</v>
+      </c>
+      <c r="E22" s="4"/>
+    </row>
+    <row r="23" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>64</v>
       </c>
@@ -5480,10 +5525,11 @@
         <v>66</v>
       </c>
       <c r="D23" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+        <v>653</v>
+      </c>
+      <c r="E23" s="4"/>
+    </row>
+    <row r="24" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>67</v>
       </c>
@@ -5494,10 +5540,11 @@
         <v>69</v>
       </c>
       <c r="D24" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+        <v>653</v>
+      </c>
+      <c r="E24" s="4"/>
+    </row>
+    <row r="25" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>70</v>
       </c>
@@ -5510,8 +5557,9 @@
       <c r="D25" t="s">
         <v>654</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E25" s="4"/>
+    </row>
+    <row r="26" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>73</v>
       </c>
@@ -5524,6 +5572,7 @@
       <c r="D26" t="s">
         <v>652</v>
       </c>
+      <c r="E26" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5532,377 +5581,633 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6B17FF2-E363-4C4C-8ED9-1567F4CA2C2F}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:P40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>655</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="5" t="s">
         <v>651</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="6" t="s">
         <v>652</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="6" t="s">
+        <v>653</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>653</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>652</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>652</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>652</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>652</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>652</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+    </row>
+    <row r="10" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>652</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+    </row>
+    <row r="11" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>652</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+    </row>
+    <row r="12" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>652</v>
+      </c>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+    </row>
+    <row r="13" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+    </row>
+    <row r="14" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>652</v>
+      </c>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+    </row>
+    <row r="15" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>652</v>
+      </c>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+    </row>
+    <row r="16" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>652</v>
+      </c>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="4"/>
+    </row>
+    <row r="17" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>652</v>
+      </c>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="4"/>
+    </row>
+    <row r="18" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>652</v>
+      </c>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+      <c r="P18" s="4"/>
+    </row>
+    <row r="19" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>652</v>
+      </c>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="4"/>
+    </row>
+    <row r="20" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>652</v>
+      </c>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="4"/>
+    </row>
+    <row r="21" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+      <c r="O21" s="4"/>
+      <c r="P21" s="4"/>
+    </row>
+    <row r="22" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B22" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="C22" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>652</v>
+      </c>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+      <c r="O22" s="4"/>
+      <c r="P22" s="4"/>
+    </row>
+    <row r="23" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D23" s="6" t="s">
         <v>653</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
+      <c r="N23" s="4"/>
+      <c r="O23" s="4"/>
+      <c r="P23" s="4"/>
+    </row>
+    <row r="24" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D24" s="6" t="s">
         <v>652</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4"/>
+      <c r="M24" s="4"/>
+      <c r="N24" s="4"/>
+      <c r="O24" s="4"/>
+      <c r="P24" s="4"/>
+    </row>
+    <row r="25" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="4"/>
+      <c r="O25" s="4"/>
+      <c r="P25" s="4"/>
+    </row>
+    <row r="26" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D26" s="6" t="s">
         <v>652</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" t="s">
-        <v>41</v>
-      </c>
-      <c r="D14" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>42</v>
-      </c>
-      <c r="B15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>45</v>
-      </c>
-      <c r="B16" t="s">
-        <v>46</v>
-      </c>
-      <c r="C16" t="s">
-        <v>47</v>
-      </c>
-      <c r="D16" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>48</v>
-      </c>
-      <c r="B17" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" t="s">
-        <v>50</v>
-      </c>
-      <c r="D17" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>51</v>
-      </c>
-      <c r="B18" t="s">
-        <v>52</v>
-      </c>
-      <c r="C18" t="s">
-        <v>53</v>
-      </c>
-      <c r="D18" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>54</v>
-      </c>
-      <c r="B19" t="s">
-        <v>55</v>
-      </c>
-      <c r="C19" t="s">
-        <v>56</v>
-      </c>
-      <c r="D19" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>57</v>
-      </c>
-      <c r="B20" t="s">
-        <v>58</v>
-      </c>
-      <c r="C20" t="s">
-        <v>59</v>
-      </c>
-      <c r="D20" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>60</v>
-      </c>
-      <c r="B21" t="s">
-        <v>61</v>
-      </c>
-      <c r="C21" t="s">
-        <v>62</v>
-      </c>
-      <c r="D21" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22" t="s">
-        <v>63</v>
-      </c>
-      <c r="D22" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>64</v>
-      </c>
-      <c r="B23" t="s">
-        <v>65</v>
-      </c>
-      <c r="C23" t="s">
-        <v>66</v>
-      </c>
-      <c r="D23" t="s">
-        <v>653</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>67</v>
-      </c>
-      <c r="B24" t="s">
-        <v>68</v>
-      </c>
-      <c r="C24" t="s">
-        <v>69</v>
-      </c>
-      <c r="D24" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>70</v>
-      </c>
-      <c r="B25" t="s">
-        <v>71</v>
-      </c>
-      <c r="C25" t="s">
-        <v>72</v>
-      </c>
-      <c r="D25" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>73</v>
-      </c>
-      <c r="B26" t="s">
-        <v>74</v>
-      </c>
-      <c r="C26" t="s">
-        <v>75</v>
-      </c>
-      <c r="D26" t="s">
-        <v>652</v>
-      </c>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="4"/>
+      <c r="M26" s="4"/>
+      <c r="N26" s="4"/>
+      <c r="O26" s="4"/>
+      <c r="P26" s="4"/>
+    </row>
+    <row r="27" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="4"/>
+      <c r="O27" s="4"/>
+      <c r="P27" s="4"/>
+    </row>
+    <row r="28" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="K28" s="4"/>
+      <c r="L28" s="4"/>
+      <c r="M28" s="4"/>
+      <c r="N28" s="4"/>
+      <c r="O28" s="4"/>
+      <c r="P28" s="4"/>
+    </row>
+    <row r="29" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="K29" s="4"/>
+      <c r="L29" s="4"/>
+      <c r="M29" s="4"/>
+      <c r="N29" s="4"/>
+      <c r="O29" s="4"/>
+      <c r="P29" s="4"/>
+    </row>
+    <row r="30" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
+      <c r="M30" s="4"/>
+      <c r="N30" s="4"/>
+      <c r="O30" s="4"/>
+      <c r="P30" s="4"/>
+    </row>
+    <row r="31" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="K31" s="4"/>
+      <c r="L31" s="4"/>
+      <c r="M31" s="4"/>
+      <c r="N31" s="4"/>
+      <c r="O31" s="4"/>
+      <c r="P31" s="4"/>
+    </row>
+    <row r="32" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="K32" s="4"/>
+      <c r="L32" s="4"/>
+      <c r="M32" s="4"/>
+      <c r="N32" s="4"/>
+      <c r="O32" s="4"/>
+      <c r="P32" s="4"/>
+    </row>
+    <row r="33" spans="11:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="K33" s="4"/>
+      <c r="L33" s="4"/>
+      <c r="M33" s="4"/>
+      <c r="N33" s="4"/>
+      <c r="O33" s="4"/>
+      <c r="P33" s="4"/>
+    </row>
+    <row r="34" spans="11:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="K34" s="4"/>
+      <c r="L34" s="4"/>
+      <c r="M34" s="4"/>
+      <c r="N34" s="4"/>
+      <c r="O34" s="4"/>
+      <c r="P34" s="4"/>
+    </row>
+    <row r="35" spans="11:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="L35" s="4"/>
+      <c r="M35" s="4"/>
+      <c r="N35" s="4"/>
+      <c r="O35" s="4"/>
+      <c r="P35" s="4"/>
+    </row>
+    <row r="36" spans="11:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="L36" s="4"/>
+      <c r="M36" s="4"/>
+      <c r="N36" s="4"/>
+      <c r="O36" s="4"/>
+      <c r="P36" s="4"/>
+    </row>
+    <row r="37" spans="11:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="L37" s="4"/>
+      <c r="M37" s="4"/>
+      <c r="N37" s="4"/>
+      <c r="O37" s="4"/>
+      <c r="P37" s="4"/>
+    </row>
+    <row r="38" spans="11:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="L38" s="4"/>
+      <c r="M38" s="4"/>
+      <c r="N38" s="4"/>
+      <c r="O38" s="4"/>
+      <c r="P38" s="4"/>
+    </row>
+    <row r="39" spans="11:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="L39" s="4"/>
+      <c r="M39" s="4"/>
+      <c r="N39" s="4"/>
+      <c r="O39" s="4"/>
+      <c r="P39" s="4"/>
+    </row>
+    <row r="40" spans="11:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="L40" s="4"/>
+      <c r="M40" s="4"/>
+      <c r="N40" s="4"/>
+      <c r="O40" s="4"/>
+      <c r="P40" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>